<commit_message>
Light sensor import done. Began analyzing light sensor data.
</commit_message>
<xml_diff>
--- a/Data/LCR Biological Data.xlsx
+++ b/Data/LCR Biological Data.xlsx
@@ -6719,10 +6719,10 @@
     <t>At island just upstream of Salt Camp. 5 min kick, 5 min pick with 2 people.</t>
   </si>
   <si>
-    <t>Coyote Camp. Removal time estimated. Took down early because boat was sinking. Lost 3 traps from this boat (not currently sure which ones).</t>
-  </si>
-  <si>
     <t>Boulders Camp. Datasheet left in camp. Need to pull in Sept.</t>
+  </si>
+  <si>
+    <t>Coyote Camp. Took down early because boat was sinking. Lost 3 traps from this boat (not currently sure which ones).</t>
   </si>
 </sst>
 </file>
@@ -33959,7 +33959,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H78" sqref="H78"/>
+      <selection pane="bottomLeft" activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35825,10 +35825,10 @@
         <v>42547</v>
       </c>
       <c r="I66" s="18">
-        <v>0.75</v>
+        <v>0.75694444444444453</v>
       </c>
       <c r="J66" s="13" t="s">
-        <v>2228</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -35851,10 +35851,10 @@
         <v>42547</v>
       </c>
       <c r="I67" s="18">
-        <v>0.75</v>
+        <v>0.75694444444444453</v>
       </c>
       <c r="J67" s="13" t="s">
-        <v>2228</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -35877,10 +35877,10 @@
         <v>42547</v>
       </c>
       <c r="I68" s="18">
-        <v>0.75</v>
+        <v>0.75694444444444453</v>
       </c>
       <c r="J68" s="13" t="s">
-        <v>2228</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -35903,10 +35903,10 @@
         <v>42547</v>
       </c>
       <c r="I69" s="18">
-        <v>0.75</v>
+        <v>0.75694444444444453</v>
       </c>
       <c r="J69" s="13" t="s">
-        <v>2228</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
@@ -35929,10 +35929,10 @@
         <v>42547</v>
       </c>
       <c r="I70" s="18">
-        <v>0.75</v>
+        <v>0.75694444444444453</v>
       </c>
       <c r="J70" s="13" t="s">
-        <v>2228</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -35955,10 +35955,10 @@
         <v>42547</v>
       </c>
       <c r="I71" s="18">
-        <v>0.75</v>
+        <v>0.75694444444444453</v>
       </c>
       <c r="J71" s="13" t="s">
-        <v>2228</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
@@ -35981,10 +35981,10 @@
         <v>42547</v>
       </c>
       <c r="I72" s="18">
-        <v>0.75</v>
+        <v>0.75694444444444453</v>
       </c>
       <c r="J72" s="13" t="s">
-        <v>2228</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -36007,10 +36007,10 @@
         <v>42547</v>
       </c>
       <c r="I73" s="18">
-        <v>0.75</v>
+        <v>0.75694444444444453</v>
       </c>
       <c r="J73" s="13" t="s">
-        <v>2228</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -36093,7 +36093,7 @@
         <v>42545</v>
       </c>
       <c r="J77" s="13" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>